<commit_message>
252a noise parameter raw data checkout
</commit_message>
<xml_diff>
--- a/npcal/18may.npcal.log.xlsx
+++ b/npcal/18may.npcal.log.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5440" yWindow="2340" windowWidth="33600" windowHeight="12380" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="5620" windowWidth="33600" windowHeight="12380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -903,7 +903,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]yyyy\-mmm\-dd;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -920,6 +920,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -983,7 +991,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1006,12 +1014,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1296,8 +1307,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V229"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="J89" sqref="J89"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1317,14 +1328,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -2189,58 +2200,58 @@
         <v>~/npcal/ant_252A.LNA0.yf346-7.off.3.2018-05-24_18-45-35.dat</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A18" s="9" t="s">
+    <row r="18" spans="1:22" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="9">
+      <c r="C18" s="22">
         <v>184629</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="22" t="s">
         <v>277</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="E18" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F18" s="11" t="s">
+      <c r="F18" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="20">
         <v>25.6</v>
       </c>
-      <c r="K18" t="s">
+      <c r="K18" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="M18" t="s">
+      <c r="M18" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="N18" t="s">
+      <c r="N18" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="O18" t="str">
+      <c r="O18" s="20" t="str">
         <f t="shared" si="0"/>
         <v>cp /nfs/jbod00/spec_dump/2018-05-24_18-46-30/ant_252A_sky.dat</v>
       </c>
-      <c r="P18" t="str">
+      <c r="P18" s="20" t="str">
         <f t="shared" si="1"/>
         <v>~/npcal/ant_252A.LNA0.yf346-7.on.1.2018-05-24_18-46-30.dat</v>
       </c>
-      <c r="R18" t="str">
+      <c r="R18" s="20" t="str">
         <f t="shared" si="2"/>
         <v>cp /nfs/jbod00/spec_dump/2018-05-24_18-46-30/ant_252A_load.dat</v>
       </c>
-      <c r="S18" t="str">
+      <c r="S18" s="20" t="str">
         <f t="shared" si="3"/>
         <v>~/npcal/ant_252A.LNA0.yf346-7.on.2.2018-05-24_18-46-30.dat</v>
       </c>
-      <c r="U18" t="str">
+      <c r="U18" s="20" t="str">
         <f t="shared" si="4"/>
         <v>cp /nfs/jbod00/spec_dump/2018-05-24_18-46-30/ant_252A_diode.dat</v>
       </c>
-      <c r="V18" t="str">
+      <c r="V18" s="20" t="str">
         <f t="shared" si="5"/>
         <v>~/npcal/ant_252A.LNA0.yf346-7.on.3.2018-05-24_18-46-30.dat</v>
       </c>
@@ -5603,55 +5614,55 @@
         <v>~/npcal/ant_254B.SW0.yf346-7.on.hotpath.2018-05-24_15-52-16.dat</v>
       </c>
     </row>
-    <row r="79" spans="1:22" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="19" t="s">
+    <row r="79" spans="1:22" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B79" s="20" t="s">
+      <c r="B79" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="C79" s="19">
+      <c r="C79" s="18">
         <v>153637</v>
       </c>
-      <c r="D79" s="19" t="s">
+      <c r="D79" s="18" t="s">
         <v>284</v>
       </c>
-      <c r="E79" s="19" t="s">
+      <c r="E79" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="F79" s="19" t="s">
+      <c r="F79" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="G79" s="21">
+      <c r="G79" s="20">
         <v>30.8</v>
       </c>
-      <c r="K79" s="21" t="s">
+      <c r="K79" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="M79" s="21" t="s">
+      <c r="M79" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="O79" s="21" t="str">
+      <c r="O79" s="20" t="str">
         <f t="shared" si="6"/>
         <v>cp /nfs/jbod00/spec_dump/2018-05-24_15-36-57/ant_254B_sky.dat</v>
       </c>
-      <c r="P79" s="21" t="str">
+      <c r="P79" s="20" t="str">
         <f t="shared" si="7"/>
         <v>~/npcal/ant_254B.SW0.2p0m.OPEN.skypath.2018-05-24_15-36-57.dat</v>
       </c>
-      <c r="R79" s="21" t="str">
+      <c r="R79" s="20" t="str">
         <f t="shared" si="8"/>
         <v>cp /nfs/jbod00/spec_dump/2018-05-24_15-36-57/ant_254B_load.dat</v>
       </c>
-      <c r="S79" s="21" t="str">
+      <c r="S79" s="20" t="str">
         <f t="shared" si="9"/>
         <v>~/npcal/ant_254B.SW0.2p0m.OPEN.coldpath.2018-05-24_15-36-57.dat</v>
       </c>
-      <c r="U79" s="21" t="str">
+      <c r="U79" s="20" t="str">
         <f t="shared" si="10"/>
         <v>cp /nfs/jbod00/spec_dump/2018-05-24_15-36-57/ant_254B_diode.dat</v>
       </c>
-      <c r="V79" s="21" t="str">
+      <c r="V79" s="20" t="str">
         <f t="shared" si="11"/>
         <v>~/npcal/ant_254B.SW0.2p0m.OPEN.hotpath.2018-05-24_15-36-57.dat</v>
       </c>
@@ -6030,117 +6041,117 @@
         <v>~/npcal/ant_254B.SW0.0p9m.TERM.hotpath.2018-05-24_16-17-03.dat</v>
       </c>
     </row>
-    <row r="87" spans="1:22" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="19" t="s">
+    <row r="87" spans="1:22" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B87" s="20" t="s">
+      <c r="B87" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="C87" s="19">
+      <c r="C87" s="18">
         <v>161850</v>
       </c>
-      <c r="D87" s="19" t="s">
+      <c r="D87" s="18" t="s">
         <v>278</v>
       </c>
-      <c r="E87" s="19" t="s">
+      <c r="E87" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="F87" s="19" t="s">
+      <c r="F87" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="G87" s="21">
+      <c r="G87" s="20">
         <v>30.5</v>
       </c>
-      <c r="J87" s="21" t="s">
+      <c r="J87" s="20" t="s">
         <v>287</v>
       </c>
-      <c r="K87" s="21" t="s">
+      <c r="K87" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="M87" s="21" t="s">
+      <c r="M87" s="20" t="s">
         <v>132</v>
       </c>
-      <c r="O87" s="21" t="str">
+      <c r="O87" s="20" t="str">
         <f t="shared" si="6"/>
         <v>cp /nfs/jbod00/spec_dump/2018-05-24_16-18-57/ant_254B_sky.dat</v>
       </c>
-      <c r="P87" s="21" t="str">
+      <c r="P87" s="20" t="str">
         <f t="shared" si="7"/>
         <v>~/npcal/ant_254B.SW0.0p9m.47pf.skypath.2018-05-24_16-18-57.dat</v>
       </c>
-      <c r="R87" s="21" t="str">
+      <c r="R87" s="20" t="str">
         <f t="shared" si="8"/>
         <v>cp /nfs/jbod00/spec_dump/2018-05-24_16-18-57/ant_254B_load.dat</v>
       </c>
-      <c r="S87" s="21" t="str">
+      <c r="S87" s="20" t="str">
         <f t="shared" si="9"/>
         <v>~/npcal/ant_254B.SW0.0p9m.47pf.coldpath.2018-05-24_16-18-57.dat</v>
       </c>
-      <c r="U87" s="21" t="str">
+      <c r="U87" s="20" t="str">
         <f t="shared" si="10"/>
         <v>cp /nfs/jbod00/spec_dump/2018-05-24_16-18-57/ant_254B_diode.dat</v>
       </c>
-      <c r="V87" s="21" t="str">
+      <c r="V87" s="20" t="str">
         <f t="shared" si="11"/>
         <v>~/npcal/ant_254B.SW0.0p9m.47pf.hotpath.2018-05-24_16-18-57.dat</v>
       </c>
     </row>
-    <row r="88" spans="1:22" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="19" t="s">
+    <row r="88" spans="1:22" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B88" s="20" t="s">
+      <c r="B88" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="C88" s="19">
+      <c r="C88" s="18">
         <v>161955</v>
       </c>
-      <c r="D88" s="19" t="s">
+      <c r="D88" s="18" t="s">
         <v>278</v>
       </c>
-      <c r="E88" s="19" t="s">
+      <c r="E88" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="F88" s="19" t="s">
+      <c r="F88" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="G88" s="21">
+      <c r="G88" s="20">
         <v>30.1</v>
       </c>
-      <c r="J88" s="21" t="s">
+      <c r="J88" s="20" t="s">
         <v>288</v>
       </c>
-      <c r="K88" s="21" t="s">
+      <c r="K88" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="M88" s="21" t="s">
+      <c r="M88" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="N88" s="21" t="s">
+      <c r="N88" s="20" t="s">
         <v>134</v>
       </c>
-      <c r="O88" s="21" t="str">
+      <c r="O88" s="20" t="str">
         <f t="shared" si="6"/>
         <v>cp /nfs/jbod00/spec_dump/2018-05-24_16-19-56/ant_254B_sky.dat</v>
       </c>
-      <c r="P88" s="21" t="str">
+      <c r="P88" s="20" t="str">
         <f t="shared" si="7"/>
         <v>~/npcal/ant_254B.SW0.0p9m.66pf.skypath.2018-05-24_16-19-56.dat</v>
       </c>
-      <c r="R88" s="21" t="str">
+      <c r="R88" s="20" t="str">
         <f t="shared" si="8"/>
         <v>cp /nfs/jbod00/spec_dump/2018-05-24_16-19-56/ant_254B_load.dat</v>
       </c>
-      <c r="S88" s="21" t="str">
+      <c r="S88" s="20" t="str">
         <f t="shared" si="9"/>
         <v>~/npcal/ant_254B.SW0.0p9m.66pf.coldpath.2018-05-24_16-19-56.dat</v>
       </c>
-      <c r="U88" s="21" t="str">
+      <c r="U88" s="20" t="str">
         <f t="shared" si="10"/>
         <v>cp /nfs/jbod00/spec_dump/2018-05-24_16-19-56/ant_254B_diode.dat</v>
       </c>
-      <c r="V88" s="21" t="str">
+      <c r="V88" s="20" t="str">
         <f t="shared" si="11"/>
         <v>~/npcal/ant_254B.SW0.0p9m.66pf.hotpath.2018-05-24_16-19-56.dat</v>
       </c>

</xml_diff>